<commit_message>
Entrega Contribución - Final
</commit_message>
<xml_diff>
--- a/docs/2023-20 Entrega 2 Pry - Declaración de la contribución.xlsx
+++ b/docs/2023-20 Entrega 2 Pry - Declaración de la contribución.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaelt\Documents\SISTRANS\B9\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E28B31D-6849-4858-B771-99D36AB92646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0239736-0577-49C1-9190-B04F973A27B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F803696E-E5CC-470A-8D77-38C02B7EB843}"/>
   </bookViews>
@@ -158,9 +158,6 @@
     <t>Así por ejemplo si un estudiante tiene una contribución del 16,66% (es decir, hizo la mitad de lo que se esperaba de él), y su grupo sacó 5.0, este estudiante obtendría una nota de 2,5 (la mitad de la nota del grupo).</t>
   </si>
   <si>
-    <t>Ana Sofia Rozo</t>
-  </si>
-  <si>
     <t>Nicolás Camargo</t>
   </si>
   <si>
@@ -168,6 +165,9 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>Adriana Sofia Rozo</t>
   </si>
 </sst>
 </file>
@@ -672,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09361F38-CEDE-46D2-A383-C99660BAC758}">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -720,13 +720,13 @@
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="D7" s="8" t="s">
         <v>41</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -742,13 +742,13 @@
         <v>9</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -756,13 +756,13 @@
         <v>10</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -778,13 +778,13 @@
         <v>12</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -802,7 +802,7 @@
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -812,7 +812,7 @@
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -822,7 +822,7 @@
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -832,7 +832,7 @@
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -840,7 +840,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
@@ -850,7 +850,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
@@ -860,7 +860,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
@@ -870,7 +870,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -881,7 +881,7 @@
       </c>
       <c r="B22" s="7"/>
       <c r="C22" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D22" s="7"/>
     </row>
@@ -891,7 +891,7 @@
       </c>
       <c r="B23" s="7"/>
       <c r="C23" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D23" s="7"/>
     </row>
@@ -901,7 +901,7 @@
       </c>
       <c r="B24" s="7"/>
       <c r="C24" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D24" s="7"/>
     </row>
@@ -911,7 +911,7 @@
       </c>
       <c r="B25" s="7"/>
       <c r="C25" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D25" s="7"/>
     </row>
@@ -929,7 +929,7 @@
       </c>
       <c r="B27" s="7"/>
       <c r="C27" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D27" s="7"/>
     </row>
@@ -938,13 +938,13 @@
         <v>28</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -970,7 +970,7 @@
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -980,7 +980,7 @@
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -990,7 +990,7 @@
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
       <c r="D33" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -1000,7 +1000,7 @@
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -1008,7 +1008,7 @@
         <v>18</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
@@ -1018,7 +1018,7 @@
         <v>19</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
@@ -1028,7 +1028,7 @@
         <v>20</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
@@ -1038,7 +1038,7 @@
         <v>21</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
@@ -1049,7 +1049,7 @@
       </c>
       <c r="B39" s="7"/>
       <c r="C39" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D39" s="7"/>
     </row>
@@ -1059,7 +1059,7 @@
       </c>
       <c r="B40" s="7"/>
       <c r="C40" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D40" s="7"/>
     </row>
@@ -1069,7 +1069,7 @@
       </c>
       <c r="B41" s="7"/>
       <c r="C41" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D41" s="7"/>
     </row>
@@ -1079,7 +1079,7 @@
       </c>
       <c r="B42" s="7"/>
       <c r="C42" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D42" s="7"/>
     </row>
@@ -1088,13 +1088,13 @@
         <v>31</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -1116,13 +1116,13 @@
         <v>33</v>
       </c>
       <c r="B45" s="15">
-        <v>0.34</v>
+        <v>0.33339999999999997</v>
       </c>
       <c r="C45" s="15">
-        <v>0.33</v>
+        <v>0.33329999999999999</v>
       </c>
       <c r="D45" s="15">
-        <v>0.33</v>
+        <v>0.33329999999999999</v>
       </c>
       <c r="E45" s="16">
         <f>SUM(B45:D47)</f>
@@ -1187,21 +1187,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010020F529DEB8C6B848B5973A83F61ADED3" ma:contentTypeVersion="7" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="4a9bcd9e3e76677356288316930ed140">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3e454257-1727-4a9d-9c89-66a9b64f5006" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="847a1593ea42407b13ba92d222becb45" ns2:_="">
     <xsd:import namespace="3e454257-1727-4a9d-9c89-66a9b64f5006"/>
@@ -1363,24 +1348,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71349ADA-141F-4CF7-8BFF-E7FB81A0DECC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70B62CA1-A0FE-45AF-BF09-3FC6FE23BC46}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F2F76ED-DFA4-43A4-9235-7004A5DFE895}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1396,4 +1379,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70B62CA1-A0FE-45AF-BF09-3FC6FE23BC46}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71349ADA-141F-4CF7-8BFF-E7FB81A0DECC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>